<commit_message>
Resolve "Extend and Test Data Import and Export"
</commit_message>
<xml_diff>
--- a/docs/assets/User Import Template.xlsx
+++ b/docs/assets/User Import Template.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Import users into Ent" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - User Import Template" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
-    <t>Import users into EntE</t>
+    <t>User Import Template</t>
   </si>
   <si>
     <t>username</t>
@@ -35,6 +34,9 @@
     <t>isAdult</t>
   </si>
   <si>
+    <t>graduationYear</t>
+  </si>
+  <si>
     <t>children</t>
   </si>
 </sst>
@@ -45,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -56,25 +58,13 @@
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -87,16 +77,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -105,28 +95,28 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -141,19 +131,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -172,7 +162,6 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
@@ -1236,16 +1225,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.35156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.17188" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.35156" style="1" customWidth="1"/>
+    <col min="9" max="256" width="8.35156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1258,224 +1252,39 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
+    <row r="2" ht="20.05" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" t="s" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="H2" t="s" s="5">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>